<commit_message>
changed source files,script and diagram
</commit_message>
<xml_diff>
--- a/Task_1_1_1/heapsort_complexity.xlsx
+++ b/Task_1_1_1/heapsort_complexity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniil\OOP\Task_1_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE51846-6E14-4626-AC60-E75E89A84B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF82EB-94E3-4224-BB1D-232DA9565D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>10^6</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>9*10^6</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>time(ms)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +345,7 @@
                   <c:v>2804</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3072</c:v>
+                  <c:v>3752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1382,14 +1388,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="K2:L27"/>
+  <dimension ref="K1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="1" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="2" spans="11:12" x14ac:dyDescent="0.35">
       <c r="K2">
         <v>1</v>
@@ -1595,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>3072</v>
+        <v>3752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>